<commit_message>
Metodo de Get y Get id funcionales
</commit_message>
<xml_diff>
--- a/cinetecbase/salas.xlsx
+++ b/cinetecbase/salas.xlsx
@@ -1,27 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Documentos\ProyectoBasesDatos\cinemaTec\cinetecbase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BC804D-8186-4349-A0C3-80E74118ED77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Salas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +356,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E9" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
post funcional y get de id con problemas
</commit_message>
<xml_diff>
--- a/cinetecbase/salas.xlsx
+++ b/cinetecbase/salas.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Salas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,9 +35,27 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>SALAMax1</t>
+  </si>
+  <si>
+    <t>Sucursal Cartago</t>
+  </si>
+  <si>
+    <t>SALA123</t>
+  </si>
+  <si>
+    <t>sala1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,7 +94,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
@@ -365,7 +383,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -390,13 +408,65 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="M5" s="1"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="E9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0">
+        <v>10</v>
+      </c>
+      <c r="D10" s="0">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0">
+        <v>10</v>
+      </c>
+      <c r="D11" s="0">
+        <v>8</v>
+      </c>
+      <c r="E11" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0">
+        <v>10</v>
+      </c>
+      <c r="D12" s="0">
+        <v>8</v>
+      </c>
+      <c r="E12" s="0">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
post y put funcionando, bug para detectar el id
</commit_message>
<xml_diff>
--- a/cinetecbase/salas.xlsx
+++ b/cinetecbase/salas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\OneDrive\Documentos\ProyectoBasesDatos\cinemaTec\cinetecbase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BC804D-8186-4349-A0C3-80E74118ED77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55719474-5F36-4E63-B3E7-1AE47793CC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,18 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>SALAMax1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Sucursal Cartago</t>
-  </si>
-  <si>
-    <t>SALA123</t>
-  </si>
-  <si>
-    <t>sala1</t>
   </si>
 </sst>
 </file>
@@ -375,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,53 +406,36 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="0">
         <v>0</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
+        <v>8</v>
+      </c>
+      <c r="D10" s="0">
         <v>10</v>
-      </c>
-      <c r="D10" s="0">
-        <v>8</v>
       </c>
       <c r="E10" s="0">
         <v>80</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>2</v>
+      <c r="A11" s="0">
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
+        <v>8</v>
+      </c>
+      <c r="D11" s="0">
         <v>10</v>
       </c>
-      <c r="D11" s="0">
-        <v>8</v>
-      </c>
       <c r="E11" s="0">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0">
-        <v>10</v>
-      </c>
-      <c r="D12" s="0">
-        <v>8</v>
-      </c>
-      <c r="E12" s="0">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego el metodo de put, detele y post a la sala controller
</commit_message>
<xml_diff>
--- a/cinetecbase/salas.xlsx
+++ b/cinetecbase/salas.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -439,6 +439,40 @@
         <v>80</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0">
+        <v>8</v>
+      </c>
+      <c r="D12" s="0">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>